<commit_message>
1_digits to black and white
</commit_message>
<xml_diff>
--- a/projection-method/output/1_digits.xlsx
+++ b/projection-method/output/1_digits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\bigbrother\projection-method\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\workspace\bigbrother\projection-method\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5953DA09-EEB5-444F-98B7-368A34EC61F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC6E40-E062-4869-A384-E0D590D4F08A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="30720" windowHeight="13296" xr2:uid="{76B1876D-A0E9-466B-BFE8-31874BF3DCB4}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="30936" windowHeight="16896" xr2:uid="{76B1876D-A0E9-466B-BFE8-31874BF3DCB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>Baseline</t>
   </si>
   <si>
-    <t>Big Brother</t>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -214,15 +214,15 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Big Brother</c:v>
+                  <c:v>Model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -230,14 +230,14 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="6350">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -343,9 +343,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="sq">
+            <a:ln w="25400" cap="sq">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
               <a:round/>
@@ -354,14 +356,18 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="6350">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -414,7 +420,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1626,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057AEF7-ED5D-4FAD-963A-C1A5AD821648}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>